<commit_message>
Fixed BTWorkCapacity, BTCrossCapacity, ACGenEnergy
</commit_message>
<xml_diff>
--- a/docs/KOSTAL_ModBus_Specifications.xlsx
+++ b/docs/KOSTAL_ModBus_Specifications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\Symcon\modules\JoT.KPP\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0C1DE8-7710-4A14-8B1E-314474F56D3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2874B6E8-4819-4472-815E-83D13FE2CDC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="20" windowWidth="18960" windowHeight="11330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="356">
   <si>
     <r>
       <rPr>
@@ -2051,6 +2051,167 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFEBEDED"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FFEBEDED"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFEBEDED"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFEBEDED"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFEBEDED"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFEBEDED"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFEBEDED"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFEBEDED"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFEBEDED"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFEBEDED"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFEBEDED"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFEBEDED"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFEBEDED"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFEBEDED"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFEBEDED"/>
+        </bottom>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="165" formatCode="0.000;[Red]0.000"/>
       <fill>
         <patternFill patternType="none">
@@ -2076,6 +2237,423 @@
         <horizontal/>
       </border>
       <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.000;[Red]0.000"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFEBEDED"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFEBEDED"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFEBEDED"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFEBEDED"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFEBEDED"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFEBEDED"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFEBEDED"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFEBEDED"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFEBEDED"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFEBEDED"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFEBEDED"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFEBEDED"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFEBEDED"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFEBEDED"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFEBEDED"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFEBEDED"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFEBEDED"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFEBEDED"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFEBEDED"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFEBEDED"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFEBEDED"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFEBEDED"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFEBEDED"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFEBEDED"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FFEBEDED"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFEBEDED"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFEBEDED"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFEBEDED"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FFEBEDED"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFEBEDED"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFEBEDED"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FFEBEDED"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FFEBEDED"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFEBEDED"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFEBEDED"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFEBEDED"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FFEBEDED"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FFEBEDED"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFEBEDED"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2137,584 +2715,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFEBEDED"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FFEBEDED"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFEBEDED"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFEBEDED"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFEBEDED"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFEBEDED"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFEBEDED"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFEBEDED"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFEBEDED"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFEBEDED"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFEBEDED"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0;[Red]0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFEBEDED"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFEBEDED"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFEBEDED"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFEBEDED"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="0.000;[Red]0.000"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFEBEDED"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFEBEDED"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFEBEDED"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFEBEDED"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFEBEDED"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFEBEDED"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFEBEDED"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFEBEDED"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFEBEDED"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFEBEDED"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFEBEDED"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFEBEDED"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFEBEDED"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFEBEDED"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFEBEDED"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFEBEDED"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFEBEDED"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFEBEDED"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFEBEDED"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFEBEDED"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFEBEDED"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFEBEDED"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFEBEDED"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFEBEDED"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFEBEDED"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFEBEDED"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFEBEDED"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFEBEDED"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0;[Red]0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FFEBEDED"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFEBEDED"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFEBEDED"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color rgb="FFEBEDED"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FFEBEDED"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFEBEDED"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFEBEDED"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFEBEDED"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FFEBEDED"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FFEBEDED"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFEBEDED"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2729,25 +2729,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{891475A2-4FB2-4681-B914-8DF59649A8A5}" name="Tabelle1" displayName="Tabelle1" ref="A1:M152" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{891475A2-4FB2-4681-B914-8DF59649A8A5}" name="Tabelle1" displayName="Tabelle1" ref="A1:M152" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="A1:M152" xr:uid="{67CFC5ED-3DF2-4325-8BB0-7109E22EA653}"/>
   <sortState ref="A2:M152">
     <sortCondition ref="A1:A152"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{9997AB42-D315-4920-ABD3-63BF9B542479}" name="Address" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{67E022DD-FFB2-4554-9D80-29B6AA2D8BF9}" name="Group" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{F9B93E8D-86B3-4B2B-B0F3-37EFA4BAC80F}" name="Ident" dataDxfId="16"/>
-    <tableColumn id="15" xr3:uid="{19AE23B1-4B73-425D-B057-6DA5633287A1}" name="ScaleIdent" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{D4274189-8352-4237-A5EC-8978C7CCE623}" name="Name" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{3F315A03-DBBC-4EEE-A147-0CD65AD4C555}" name="Profile" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{F24BF87B-55D8-49EA-83E7-DF00F2B87F83}" name="VarType" dataDxfId="12"/>
-    <tableColumn id="16" xr3:uid="{F1CAE169-D78E-4F13-925D-EB394D9C70FB}" name="Factor" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{8C62C676-2CC7-4D4C-B133-9A861FB7819C}" name="MBType" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{B12D7364-1EDB-440B-9FC2-31E2C3FADF6E}" name="Quantity" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{9769FDF8-F134-4F7D-97E0-9FB704DEDEAF}" name="RFunction" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{2697D931-01F8-4871-AA39-B743702F9207}" name="WFunction" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{370C0678-26F2-4D02-BE87-0190FE344869}" name="FWVersion" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{9997AB42-D315-4920-ABD3-63BF9B542479}" name="Address" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{67E022DD-FFB2-4554-9D80-29B6AA2D8BF9}" name="Group" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{F9B93E8D-86B3-4B2B-B0F3-37EFA4BAC80F}" name="Ident" dataDxfId="10"/>
+    <tableColumn id="15" xr3:uid="{19AE23B1-4B73-425D-B057-6DA5633287A1}" name="ScaleIdent" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{D4274189-8352-4237-A5EC-8978C7CCE623}" name="Name" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{3F315A03-DBBC-4EEE-A147-0CD65AD4C555}" name="Profile" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{F24BF87B-55D8-49EA-83E7-DF00F2B87F83}" name="VarType" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{F1CAE169-D78E-4F13-925D-EB394D9C70FB}" name="Factor" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{8C62C676-2CC7-4D4C-B133-9A861FB7819C}" name="MBType" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{B12D7364-1EDB-440B-9FC2-31E2C3FADF6E}" name="Quantity" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{9769FDF8-F134-4F7D-97E0-9FB704DEDEAF}" name="RFunction" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{2697D931-01F8-4871-AA39-B743702F9207}" name="WFunction" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{370C0678-26F2-4D02-BE87-0190FE344869}" name="FWVersion" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3077,8 +3077,8 @@
   <dimension ref="A1:M152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H98" sqref="H98"/>
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C139" sqref="C139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3704,7 +3704,9 @@
         <v>113</v>
       </c>
       <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
+      <c r="I20" s="19" t="s">
+        <v>355</v>
+      </c>
       <c r="J20" s="24">
         <v>2</v>
       </c>
@@ -6361,7 +6363,9 @@
         <v>113</v>
       </c>
       <c r="H99" s="19"/>
-      <c r="I99" s="19"/>
+      <c r="I99" s="19" t="s">
+        <v>355</v>
+      </c>
       <c r="J99" s="24">
         <v>2</v>
       </c>
@@ -6555,7 +6559,9 @@
       <c r="H105" s="19">
         <v>1E-3</v>
       </c>
-      <c r="I105" s="19"/>
+      <c r="I105" s="19" t="s">
+        <v>355</v>
+      </c>
       <c r="J105" s="24">
         <v>2</v>
       </c>
@@ -6827,7 +6833,9 @@
       <c r="H113" s="19">
         <v>1E-3</v>
       </c>
-      <c r="I113" s="19"/>
+      <c r="I113" s="19" t="s">
+        <v>355</v>
+      </c>
       <c r="J113" s="24">
         <v>2</v>
       </c>
@@ -8181,22 +8189,22 @@
   </sheetData>
   <sheetProtection sheet="1" insertRows="0" selectLockedCells="1" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="D122">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C152 C2:C124 C126:C146">
-    <cfRule type="duplicateValues" dxfId="5" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C149:C151">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C148">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C147">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K152" xr:uid="{44DEFA60-CD9D-49B1-9B1E-F329372B473B}">

</xml_diff>

<commit_message>
Fixed FW-Version for DeviceInfo
</commit_message>
<xml_diff>
--- a/docs/KOSTAL_ModBus_Specifications.xlsx
+++ b/docs/KOSTAL_ModBus_Specifications.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20369"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20370"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\Symcon\modules\JoT.KPP\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4FCBE8-32C7-41D2-8AEF-81B4C40B992B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDAAB9F-3BD0-480D-9ED4-792BD4BD1187}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="20" windowWidth="18960" windowHeight="11330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3077,8 +3077,8 @@
   <dimension ref="A1:M152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C99" sqref="C99"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M120" sqref="M120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3492,7 +3492,7 @@
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="5">
-        <v>1.42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
@@ -3616,7 +3616,7 @@
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="5">
-        <v>1.42</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
@@ -3649,7 +3649,7 @@
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="5">
-        <v>1.42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
@@ -6081,7 +6081,7 @@
       </c>
       <c r="L90" s="4"/>
       <c r="M90" s="5">
-        <v>1.42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.35">
@@ -6704,7 +6704,7 @@
       </c>
       <c r="L109" s="4"/>
       <c r="M109" s="5">
-        <v>1.42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.35">
@@ -7071,7 +7071,7 @@
       </c>
       <c r="L120" s="4"/>
       <c r="M120" s="5">
-        <v>1.42</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.35">
@@ -7104,7 +7104,7 @@
       </c>
       <c r="L121" s="4"/>
       <c r="M121" s="5">
-        <v>1.42</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.35">

</xml_diff>